<commit_message>
new: VIRAL exception included to handle viral's effects on opponents
</commit_message>
<xml_diff>
--- a/DoomPy/files/cards.xlsx
+++ b/DoomPy/files/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azabicki/Sync/Projects/DoomPy/DoomPy/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9C7BCD-63C3-1E4A-9B40-27419EE22764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6A127E-262A-CD42-B340-5148E072D2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="880" windowWidth="39460" windowHeight="24400" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
+    <workbookView xWindow="9420" yWindow="520" windowWidth="41600" windowHeight="26140" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
   </bookViews>
   <sheets>
     <sheet name="traits" sheetId="1" r:id="rId1"/>
@@ -1233,9 +1233,6 @@
     <t>1 self n_colorless own</t>
   </si>
   <si>
-    <t>-1 other n_color_worlds_end own</t>
-  </si>
-  <si>
     <t>-1 self n_traits own</t>
   </si>
   <si>
@@ -1269,12 +1266,6 @@
     <t>1 self n_green own</t>
   </si>
   <si>
-    <t>1 self n_green_pairs own</t>
-  </si>
-  <si>
-    <t>1 self n_hand own</t>
-  </si>
-  <si>
     <t>1 self n_purple own</t>
   </si>
   <si>
@@ -1290,9 +1281,6 @@
     <t>2 self if_green_most_traits own</t>
   </si>
   <si>
-    <t>2 self n_dominant hand</t>
-  </si>
-  <si>
     <t>2 self lowest_color_count own</t>
   </si>
   <si>
@@ -1308,9 +1296,6 @@
     <t>n self n_swarm all</t>
   </si>
   <si>
-    <t>n self hand_cards_with_effects</t>
-  </si>
-  <si>
     <t>n self n_kidney own</t>
   </si>
   <si>
@@ -1323,13 +1308,28 @@
     <t>n self n_colors own</t>
   </si>
   <si>
-    <t>n self n_hand own</t>
-  </si>
-  <si>
-    <t>1 self n_solors_hand own</t>
-  </si>
-  <si>
     <t>n self host own</t>
+  </si>
+  <si>
+    <t>2 self n_dominant own_hand</t>
+  </si>
+  <si>
+    <t>1 self n_hand own_hand</t>
+  </si>
+  <si>
+    <t>n self cards_with_effects own_hand</t>
+  </si>
+  <si>
+    <t>n self n_hand own_hand</t>
+  </si>
+  <si>
+    <t>1 self n_color_pairs own</t>
+  </si>
+  <si>
+    <t>1 self n_colors_hand own_hand</t>
+  </si>
+  <si>
+    <t>-1 opponents n_color_worlds_end own</t>
   </si>
 </sst>
 </file>
@@ -2017,8 +2017,8 @@
   <dimension ref="A1:P213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O34" sqref="O34"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2160,7 +2160,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="O4" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2246,7 +2246,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="O8" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -2444,7 +2444,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="O17" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -2619,7 +2619,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="O25" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -2668,7 +2668,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="O27" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -2694,7 +2694,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="O28" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -2800,7 +2800,7 @@
         <v>229</v>
       </c>
       <c r="O32" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -2834,7 +2834,7 @@
         <v>229</v>
       </c>
       <c r="O33" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -3003,7 +3003,7 @@
         <v>1</v>
       </c>
       <c r="O41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -3023,7 +3023,7 @@
         <v>1</v>
       </c>
       <c r="O42" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -3273,7 +3273,7 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="O54" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
@@ -3359,7 +3359,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
       <c r="O58" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -3485,7 +3485,7 @@
         <v>1</v>
       </c>
       <c r="O64" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
@@ -3771,7 +3771,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
       <c r="O76" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
@@ -3797,7 +3797,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
       <c r="O77" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
@@ -3931,7 +3931,7 @@
         <v>381</v>
       </c>
       <c r="O83" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
@@ -3962,7 +3962,7 @@
         <v>381</v>
       </c>
       <c r="O84" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
@@ -3988,7 +3988,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
       <c r="O85" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
@@ -4060,7 +4060,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
       <c r="O88" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
@@ -4162,7 +4162,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
       <c r="O92" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.2">
@@ -4204,7 +4204,7 @@
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="O94" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.2">
@@ -4371,7 +4371,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
       <c r="O101" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
@@ -4397,7 +4397,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
       <c r="O102" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
@@ -4423,7 +4423,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
       <c r="O103" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
@@ -4449,7 +4449,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
       <c r="O104" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
@@ -4475,7 +4475,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
       <c r="O105" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
@@ -4501,7 +4501,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
       <c r="O106" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
@@ -4527,7 +4527,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
       <c r="O107" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
@@ -4670,7 +4670,7 @@
         <v>380</v>
       </c>
       <c r="O113" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
@@ -4698,7 +4698,7 @@
         <v>380</v>
       </c>
       <c r="O114" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
@@ -4885,7 +4885,7 @@
         <v>379</v>
       </c>
       <c r="O122" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
@@ -4913,7 +4913,7 @@
         <v>379</v>
       </c>
       <c r="O123" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
@@ -5077,7 +5077,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
       <c r="O131" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.2">
@@ -5106,7 +5106,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
       <c r="O132" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.2">
@@ -5135,7 +5135,7 @@
       <c r="K133" s="3"/>
       <c r="L133" s="3"/>
       <c r="O133" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.2">
@@ -5299,7 +5299,7 @@
       <c r="K140" s="3"/>
       <c r="L140" s="3"/>
       <c r="O140" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.2">
@@ -5523,7 +5523,7 @@
       <c r="K151" s="3"/>
       <c r="L151" s="3"/>
       <c r="O151" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.2">
@@ -5928,7 +5928,7 @@
       <c r="K168" s="3"/>
       <c r="L168" s="3"/>
       <c r="O168" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="P168" s="23" t="s">
         <v>395</v>
@@ -5951,7 +5951,7 @@
         <v>1</v>
       </c>
       <c r="O169" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
@@ -5971,7 +5971,7 @@
         <v>1</v>
       </c>
       <c r="O170" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
@@ -6043,7 +6043,7 @@
       <c r="K173" s="3"/>
       <c r="L173" s="3"/>
       <c r="O173" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
@@ -6174,7 +6174,7 @@
       <c r="K178" s="3"/>
       <c r="L178" s="3"/>
       <c r="O178" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.2">
@@ -6200,7 +6200,7 @@
       <c r="K179" s="3"/>
       <c r="L179" s="3"/>
       <c r="O179" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.2">
@@ -6226,7 +6226,7 @@
       <c r="K180" s="3"/>
       <c r="L180" s="3"/>
       <c r="O180" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.2">
@@ -6252,7 +6252,7 @@
       <c r="K181" s="3"/>
       <c r="L181" s="3"/>
       <c r="O181" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.2">
@@ -6278,7 +6278,7 @@
       <c r="K182" s="3"/>
       <c r="L182" s="3"/>
       <c r="O182" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.2">
@@ -6304,7 +6304,7 @@
       <c r="K183" s="3"/>
       <c r="L183" s="3"/>
       <c r="O183" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.2">
@@ -6356,7 +6356,7 @@
       <c r="K185" s="3"/>
       <c r="L185" s="3"/>
       <c r="O185" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.2">
@@ -6624,7 +6624,7 @@
       <c r="K197" s="3"/>
       <c r="L197" s="3"/>
       <c r="O197" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.2">
@@ -6644,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="O198" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.2">
@@ -6843,7 +6843,7 @@
       <c r="K206" s="3"/>
       <c r="L206" s="3"/>
       <c r="O206" s="23" t="s">
-        <v>398</v>
+        <v>430</v>
       </c>
       <c r="P206" s="23" t="s">
         <v>395</v>
@@ -7008,7 +7008,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:S219">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:R219">
     <sortCondition descending="1" ref="F1:F219"/>
     <sortCondition ref="A1:A219"/>
   </sortState>

</xml_diff>

<commit_message>
littel fix in xlsx
</commit_message>
<xml_diff>
--- a/DoomPy/files/cards.xlsx
+++ b/DoomPy/files/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azabicki/Sync/Projects/DoomPy/DoomPy/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046B65A4-8078-344F-AAD6-97BCED58F7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B6799C-1C6A-5C43-806B-117A290E5C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14900" yWindow="1720" windowWidth="32620" windowHeight="21640" activeTab="2" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
   </bookViews>
@@ -2106,7 +2106,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2134,11 +2134,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2176,6 +2185,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2199,6 +2209,14 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2237,6 +2255,11 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2725,26 +2748,26 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FF236492-2866-7A4C-8166-84E97629A067}" name="Tabelle3" displayName="Tabelle3" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FF236492-2866-7A4C-8166-84E97629A067}" name="Tabelle3" displayName="Tabelle3" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
   <autoFilter ref="A1:D1048576" xr:uid="{FF236492-2866-7A4C-8166-84E97629A067}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3E8585BE-B941-1E48-9DBC-BC4A5DFA0274}" name="MOL" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{B5611C06-DB54-6747-BEE3-1D24D886F23F}" name="game" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{B76D2281-A8FA-214A-A5D4-A132C9A872EC}" name="condition_A" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{8EA65515-2984-C648-8BE8-09497BB8793B}" name="condition_B" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B5611C06-DB54-6747-BEE3-1D24D886F23F}" name="game" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B76D2281-A8FA-214A-A5D4-A132C9A872EC}" name="condition_A" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{8EA65515-2984-C648-8BE8-09497BB8793B}" name="condition_B" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{715F6A3D-646B-F247-BD73-8036CDB65C52}" name="Tabelle4" displayName="Tabelle4" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{715F6A3D-646B-F247-BD73-8036CDB65C52}" name="Tabelle4" displayName="Tabelle4" ref="A1:D1048576" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
   <autoFilter ref="A1:D1048576" xr:uid="{715F6A3D-646B-F247-BD73-8036CDB65C52}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{66C7ED80-D3EC-8F48-924C-CE8C7AC0483C}" name="MOL" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{3D25D872-9D29-3C47-8727-0E8B85603B25}" name="game" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{1E43C93B-7BA5-7D4F-81D2-60C55D1EA81E}" name="condition_A" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{B4D6E143-9614-9646-A65C-90C01526CFA4}" name="condition_B" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{66C7ED80-D3EC-8F48-924C-CE8C7AC0483C}" name="MOL" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{3D25D872-9D29-3C47-8727-0E8B85603B25}" name="game" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{1E43C93B-7BA5-7D4F-81D2-60C55D1EA81E}" name="condition_A" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{B4D6E143-9614-9646-A65C-90C01526CFA4}" name="condition_B" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16780,11 +16803,325 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB22EBC-98B5-0A4B-BE66-A269A8B9C2CC}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>613</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>616</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
+        <v>612</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>617</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>623</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>625</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>629</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>631</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>633</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>635</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>637</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>639</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>641</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>643</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>645</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>647</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="31"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="31"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="31"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="31"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C24" s="31"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C25" s="31"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C26" s="31"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C27" s="31"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C28" s="31"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C29" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF8EC9B-FEC3-8446-BCFE-151ABD0F12CA}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16820,294 +17157,6 @@
         <v>616</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
-        <v>612</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>617</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>619</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>622</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C6" s="31" t="s">
-        <v>623</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C7" s="31" t="s">
-        <v>625</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>627</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>629</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>631</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>633</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>635</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>637</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>639</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>641</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>643</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>645</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>647</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>649</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF8EC9B-FEC3-8446-BCFE-151ABD0F12CA}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.33203125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="31"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>613</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>616</v>
-      </c>
-      <c r="D2" s="31" t="s">
         <v>650</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some minor errors
</commit_message>
<xml_diff>
--- a/DoomPy/files/cards.xlsx
+++ b/DoomPy/files/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azabicki/Sync/Projects/DoomPy/DoomPy/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D6DB41-5D39-7741-813A-5275ACFAEC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2014A1A7-4F10-CE46-91B7-23A9F43674E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="3820" windowWidth="31200" windowHeight="21640" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
   </bookViews>
@@ -2881,7 +2881,13 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FF236492-2866-7A4C-8166-84E97629A067}" name="Tabelle3" displayName="Tabelle3" ref="A1:F67" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:F67" xr:uid="{FF236492-2866-7A4C-8166-84E97629A067}"/>
+  <autoFilter ref="A1:F67" xr:uid="{FF236492-2866-7A4C-8166-84E97629A067}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="MOL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F67">
     <sortCondition ref="B1:B67"/>
   </sortState>
@@ -3196,9 +3202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AE435C-BBFF-4D4C-B457-AFC1FAEE6491}">
   <dimension ref="A1:Y367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B247" sqref="B247"/>
+      <selection pane="topRight" activeCell="B246" sqref="B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17710,7 +17716,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>741</v>
       </c>
@@ -17750,7 +17756,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>742</v>
       </c>
@@ -17770,7 +17776,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>741</v>
       </c>
@@ -17790,7 +17796,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>741</v>
       </c>
@@ -17810,7 +17816,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>741</v>
       </c>
@@ -17850,7 +17856,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>742</v>
       </c>
@@ -17870,7 +17876,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>741</v>
       </c>
@@ -17890,7 +17896,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>741</v>
       </c>
@@ -17930,7 +17936,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>742</v>
       </c>
@@ -17970,7 +17976,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>742</v>
       </c>
@@ -17990,7 +17996,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>741</v>
       </c>
@@ -18010,7 +18016,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>741</v>
       </c>
@@ -18050,7 +18056,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>742</v>
       </c>
@@ -18070,7 +18076,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>741</v>
       </c>
@@ -18090,7 +18096,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>741</v>
       </c>
@@ -18110,7 +18116,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>741</v>
       </c>
@@ -18130,7 +18136,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>741</v>
       </c>
@@ -18150,7 +18156,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>741</v>
       </c>
@@ -18170,7 +18176,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>741</v>
       </c>
@@ -18210,7 +18216,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>742</v>
       </c>
@@ -18230,7 +18236,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>741</v>
       </c>
@@ -18270,7 +18276,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>742</v>
       </c>
@@ -18310,7 +18316,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>742</v>
       </c>
@@ -18330,7 +18336,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>741</v>
       </c>
@@ -18370,7 +18376,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>742</v>
       </c>
@@ -18410,7 +18416,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>742</v>
       </c>
@@ -18430,7 +18436,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>741</v>
       </c>
@@ -18450,7 +18456,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>741</v>
       </c>
@@ -18470,7 +18476,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>741</v>
       </c>
@@ -18490,7 +18496,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>741</v>
       </c>
@@ -18510,7 +18516,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>741</v>
       </c>
@@ -18530,7 +18536,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>741</v>
       </c>
@@ -18550,7 +18556,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>741</v>
       </c>
@@ -18570,7 +18576,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>741</v>
       </c>
@@ -18590,7 +18596,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>741</v>
       </c>
@@ -18630,7 +18636,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>742</v>
       </c>
@@ -18670,7 +18676,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>742</v>
       </c>
@@ -18690,7 +18696,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>741</v>
       </c>
@@ -18730,7 +18736,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>742</v>
       </c>
@@ -18750,7 +18756,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>741</v>
       </c>
@@ -18770,7 +18776,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>741</v>
       </c>
@@ -18810,7 +18816,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>742</v>
       </c>
@@ -18850,7 +18856,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>742</v>
       </c>
@@ -18890,7 +18896,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>742</v>
       </c>
@@ -18930,7 +18936,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>742</v>
       </c>
@@ -18970,7 +18976,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>742</v>
       </c>
@@ -18990,7 +18996,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>741</v>
       </c>
@@ -19010,7 +19016,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>741</v>
       </c>

</xml_diff>